<commit_message>
Detect cycle in a graph
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDF956B-F61B-4459-A8B6-D9662B3A9247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F227E2-6DFE-4BC2-9697-ED33D33C49E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="C358" sqref="C358"/>
+      <selection activeCell="B360" sqref="B360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5742,7 +5742,7 @@
       <c r="B360" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="C360" s="4" t="s">
+      <c r="C360" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Detect cycle in directed graph
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F227E2-6DFE-4BC2-9697-ED33D33C49E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8206B0F6-7898-4374-A8B9-5D8C978EF5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="B360" sqref="B360"/>
+      <selection activeCell="C359" sqref="C359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5731,7 +5731,7 @@
       <c r="B359" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="C359" s="4" t="s">
+      <c r="C359" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Topological order by BFS
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8206B0F6-7898-4374-A8B9-5D8C978EF5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF30F50B-FBF3-489F-B9D2-93DA854F38BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="C359" sqref="C359"/>
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="C368" sqref="C368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5830,7 +5830,7 @@
       <c r="B368" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C368" s="4" t="s">
+      <c r="C368" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rat in a maze
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF30F50B-FBF3-489F-B9D2-93DA854F38BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A816D22B-E070-4175-B9A4-410FDD64C201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
-      <selection activeCell="C368" sqref="C368"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="B270" sqref="B270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -4849,7 +4849,7 @@
       <c r="B275" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C275" s="4" t="s">
+      <c r="C275" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5753,7 +5753,7 @@
       <c r="B361" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="C361" s="4" t="s">
+      <c r="C361" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minimum steps by knight to reach the destination
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A816D22B-E070-4175-B9A4-410FDD64C201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCF5ACB-4148-4E6B-A4D2-7C45E6A6B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
-      <selection activeCell="B270" sqref="B270"/>
+    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
+      <selection activeCell="B363" sqref="B363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5764,7 +5764,7 @@
       <c r="B362" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="C362" s="4" t="s">
+      <c r="C362" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flood fill algorithm bfs
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCF5ACB-4148-4E6B-A4D2-7C45E6A6B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1B198B-D317-47AF-8594-F647F71500BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
-      <selection activeCell="B363" sqref="B363"/>
+      <selection activeCell="C363" sqref="C363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5775,7 +5775,7 @@
       <c r="B363" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="C363" s="4" t="s">
+      <c r="C363" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Min Number of Operations to Make Network Connected
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1B198B-D317-47AF-8594-F647F71500BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A999CB59-28D8-41AE-8658-4C1FB4F52D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
-      <selection activeCell="C363" sqref="C363"/>
+    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
+      <selection activeCell="C366" sqref="C366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5797,7 +5797,7 @@
       <c r="B365" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="C365" s="4" t="s">
+      <c r="C365" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Min time taken by each job in DAC
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A999CB59-28D8-41AE-8658-4C1FB4F52D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411A2C2E-27AA-4679-9D67-B0A277DC6736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="C366" sqref="C366"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="B364" sqref="B364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5841,7 +5841,7 @@
       <c r="B369" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C369" s="4" t="s">
+      <c r="C369" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Find number of islands
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411A2C2E-27AA-4679-9D67-B0A277DC6736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED0C4E9-8C05-4236-B428-8C6EC541B8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
-      <selection activeCell="B364" sqref="B364"/>
+      <selection activeCell="B366" sqref="B366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5863,7 +5863,7 @@
       <c r="B371" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="C371" s="4" t="s">
+      <c r="C371" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
possiblility to finish all tasks or not from given dependencies
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED0C4E9-8C05-4236-B428-8C6EC541B8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B092164-DD95-4CBB-A88C-182047C31AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
-      <selection activeCell="B366" sqref="B366"/>
+      <selection activeCell="C370" sqref="C370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5852,7 +5852,7 @@
       <c r="B370" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="C370" s="4" t="s">
+      <c r="C370" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implementation of Dijkstra Algo
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B092164-DD95-4CBB-A88C-182047C31AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91EFB52-9DC9-4972-B855-818E4BBF2108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
-      <selection activeCell="C370" sqref="C370"/>
+    <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
+      <selection activeCell="C367" sqref="C367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5819,7 +5819,7 @@
       <c r="B367" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="C367" s="4" t="s">
+      <c r="C367" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Kruskal algo using disjoint set.
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF811FB-7D8B-44F3-9B9E-CC58EFE1FEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D973C343-59E5-402C-A0D1-15F710D551C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" workbookViewId="0">
-      <selection activeCell="B374" sqref="B374"/>
+    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
+      <selection activeCell="C373" sqref="C373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5885,7 +5885,7 @@
       <c r="B373" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="C373" s="4" t="s">
+      <c r="C373" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Snake and Ladder Using BFS
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D973C343-59E5-402C-A0D1-15F710D551C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ACDF8A-D9C0-45E1-B5DC-6D93DB197605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
-      <selection activeCell="C373" sqref="C373"/>
+    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
+      <selection activeCell="B374" sqref="B374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5962,7 +5962,7 @@
       <c r="B380" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="C380" s="4" t="s">
+      <c r="C380" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Journey to the moon using disjoint set ds
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ACDF8A-D9C0-45E1-B5DC-6D93DB197605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301DF9AB-4A93-4D62-B431-C65F231D390B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="476">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1450,6 +1450,9 @@
   </si>
   <si>
     <t>using DP soln</t>
+  </si>
+  <si>
+    <t>did using Disjoint Set, try dfs method</t>
   </si>
 </sst>
 </file>
@@ -1969,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="B374" sqref="B374"/>
+    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
+      <selection activeCell="B389" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6021,15 +6024,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="386" spans="1:3" ht="21">
+    <row r="386" spans="1:3" ht="32.4">
       <c r="A386" s="8" t="s">
         <v>343</v>
       </c>
       <c r="B386" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="C386" s="4" t="s">
-        <v>4</v>
+      <c r="C386" s="20" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="387" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Detect Negative Cycle in a Graph using Bellman-Ford algo
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26BB52C-27FC-4A41-B107-E1AE042A93BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C773D1-FA1F-43D3-A979-926B40343C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="B376" sqref="B376"/>
+    <sheetView tabSelected="1" topLeftCell="A378" workbookViewId="0">
+      <selection activeCell="C384" sqref="C384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6009,7 +6009,7 @@
       <c r="B384" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C384" s="4" t="s">
+      <c r="C384" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Path more than k length from source
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5A39FC-A23E-45AE-BE60-30C8FC1A1FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600B1AEB-E433-4AFA-8CED-D2A5FD8C6F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
-      <selection activeCell="C382" sqref="C382"/>
+    <sheetView tabSelected="1" topLeftCell="A383" workbookViewId="0">
+      <selection activeCell="B389" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5954,7 +5954,7 @@
       <c r="B379" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="C379" s="4" t="s">
+      <c r="C379" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6086,7 +6086,7 @@
       <c r="B391" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="C391" s="4" t="s">
+      <c r="C391" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Oliver and Game - Euler Tour
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600B1AEB-E433-4AFA-8CED-D2A5FD8C6F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEB35E8-1CBD-45F2-BC0F-1E2A12D62DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A383" workbookViewId="0">
-      <selection activeCell="B389" sqref="B389"/>
+      <selection activeCell="B386" sqref="B386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6053,7 +6053,7 @@
       <c r="B388" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="C388" s="4" t="s">
+      <c r="C388" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
M coloring using Backtracking
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEB35E8-1CBD-45F2-BC0F-1E2A12D62DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC34F83-59A1-49D7-8AD6-DE651FE7A69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A383" workbookViewId="0">
-      <selection activeCell="B386" sqref="B386"/>
+    <sheetView tabSelected="1" topLeftCell="A380" workbookViewId="0">
+      <selection activeCell="B389" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -6097,7 +6097,7 @@
       <c r="B392" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="C392" s="4" t="s">
+      <c r="C392" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Check wheather graph is bipartite or not
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC34F83-59A1-49D7-8AD6-DE651FE7A69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DA7517-818C-4AE3-8036-B19FB23BB5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="B389" sqref="B389"/>
+    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
+      <selection activeCell="C383" sqref="C383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5998,7 +5998,7 @@
       <c r="B383" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C383" s="4" t="s">
+      <c r="C383" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Connect N Ropes With Minimum Cost
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC852981-A25F-48E9-888B-2B74A4BD384A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB655F5-4A95-429A-8D53-F3A2F20147A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
-      <selection activeCell="C341" sqref="C341"/>
+      <selection activeCell="C349" sqref="C349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5638,7 +5638,7 @@
       <c r="B349" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C349" s="4" t="s">
+      <c r="C349" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Check strings are rotations of each other
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10398EEE-0E4A-48AC-9095-C73630EFFF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7555AC82-FB90-4B0E-898C-077913167919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="C344" sqref="C344"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2584,7 +2584,7 @@
       <c r="B60" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Find all permuations of a string in lexicographical order
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7555AC82-FB90-4B0E-898C-077913167919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA20B020-0F8A-4F0F-AE75-1B5B16E464C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2650,7 +2650,7 @@
       <c r="B66" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Print all subsequence of a string
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA20B020-0F8A-4F0F-AE75-1B5B16E464C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC401E2-70E3-4FA9-A7EC-31C30C62CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2639,7 +2639,7 @@
       <c r="B65" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
count unique binary string into equal 0 and 1
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC401E2-70E3-4FA9-A7EC-31C30C62CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E945DC5C-850A-4118-BA86-5A694DC56667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2661,7 +2661,7 @@
       <c r="B67" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minimum op to transform string by shifting them at the back
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DE3792-0C2F-4D8B-8725-C08AB2BD4F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5ACE90-27FB-480A-AFEC-E904EE1821B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2980,7 +2980,7 @@
       <c r="B96" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minimum reversal of bracket to make expression balanced
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5ACE90-27FB-480A-AFEC-E904EE1821B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4271CC04-ACC8-4330-9DD1-AEA5D65FC8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2760,7 +2760,7 @@
       <c r="B76" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minimum flips to alternate binary strings
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4271CC04-ACC8-4330-9DD1-AEA5D65FC8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E612C2-6169-48D1-8A39-FEB8326B2B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1972,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2837,7 +2837,7 @@
       <c r="B83" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C83" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Second most repeated string
</commit_message>
<xml_diff>
--- a/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
+++ b/Classic Problems/Babbar DSA sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAXMAN\Desktop\DSA\Classic Problems\Babbar DSA sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E612C2-6169-48D1-8A39-FEB8326B2B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99CC8D2-AE48-431B-9253-1ACB1DAC703A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1973,7 +1973,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2848,7 +2848,7 @@
       <c r="B84" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>